<commit_message>
Implemented google calendar and improved display issues
</commit_message>
<xml_diff>
--- a/storage/imports/cities.xlsx
+++ b/storage/imports/cities.xlsx
@@ -1021,7 +1021,7 @@
     <t>VENTAQUEMADA</t>
   </si>
   <si>
-    <t>VILLA DE LEIVA</t>
+    <t>VILLA DE LEYVA</t>
   </si>
   <si>
     <t xml:space="preserve">VIRACACHA </t>
@@ -3125,7 +3125,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000000000000"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -3140,6 +3140,10 @@
       <sz val="11.0"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="Cambria"/>
     </font>
   </fonts>
   <fills count="2">
@@ -3156,7 +3160,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -3168,6 +3172,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -11044,7 +11051,7 @@
         <v>-73525.0</v>
       </c>
       <c r="D333" s="1"/>
-      <c r="E333" s="1" t="s">
+      <c r="E333" s="4" t="s">
         <v>336</v>
       </c>
       <c r="F333" s="1"/>
@@ -29135,26 +29142,26 @@
       </c>
     </row>
     <row r="1120" ht="12.75" customHeight="1">
-      <c r="A1120" s="4"/>
+      <c r="A1120" s="5"/>
       <c r="B1120" s="2"/>
       <c r="C1120" s="2"/>
-      <c r="D1120" s="4"/>
-      <c r="E1120" s="4"/>
-      <c r="F1120" s="4"/>
-      <c r="G1120" s="4"/>
-      <c r="H1120" s="4"/>
-      <c r="I1120" s="4"/>
+      <c r="D1120" s="5"/>
+      <c r="E1120" s="5"/>
+      <c r="F1120" s="5"/>
+      <c r="G1120" s="5"/>
+      <c r="H1120" s="5"/>
+      <c r="I1120" s="5"/>
     </row>
     <row r="1121" ht="12.75" customHeight="1">
-      <c r="A1121" s="4"/>
+      <c r="A1121" s="5"/>
       <c r="B1121" s="2"/>
       <c r="C1121" s="2"/>
-      <c r="D1121" s="4"/>
-      <c r="E1121" s="4"/>
-      <c r="F1121" s="4"/>
-      <c r="G1121" s="4"/>
-      <c r="H1121" s="4"/>
-      <c r="I1121" s="4"/>
+      <c r="D1121" s="5"/>
+      <c r="E1121" s="5"/>
+      <c r="F1121" s="5"/>
+      <c r="G1121" s="5"/>
+      <c r="H1121" s="5"/>
+      <c r="I1121" s="5"/>
     </row>
   </sheetData>
   <printOptions/>

</xml_diff>